<commit_message>
Update Check pearson correlation
</commit_message>
<xml_diff>
--- a/database/classified_reaction_types/ketone_alcohol/ketone_alcohol_6C_test.xlsx
+++ b/database/classified_reaction_types/ketone_alcohol/ketone_alcohol_6C_test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Reactants</t>
   </si>
@@ -27,14 +27,6 @@
     <t>Products</t>
   </si>
   <si>
-    <t>Types</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Angle</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>O=CCc1ccccc1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -73,6 +65,24 @@
   <si>
     <t>CCc1ccc(cc1)CO</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The closest predicted product</t>
+  </si>
+  <si>
+    <t>OCCCc1ccccc1</t>
+  </si>
+  <si>
+    <t>OCCCc1cccc(c1)C(=O)C</t>
+  </si>
+  <si>
+    <t>OCC(c1ccccc1CC)C</t>
+  </si>
+  <si>
+    <t>OCC(c1ccc(cc1)CC)C</t>
+  </si>
+  <si>
+    <t>OCCc1ccc(cc1)CC</t>
   </si>
 </sst>
 </file>
@@ -403,14 +413,14 @@
   <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.375" customWidth="1"/>
     <col min="2" max="2" width="28.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -422,53 +432,62 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>